<commit_message>
Changed aside files as I'm reinstalling os.
</commit_message>
<xml_diff>
--- a/aside/qm/chap2.xlsx
+++ b/aside/qm/chap2.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem Batutin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem Batutin\Documents\school\champ\aside\qm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" tabRatio="328"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" tabRatio="328" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="intro" sheetId="1" r:id="rId1"/>
+    <sheet name="3.2_#6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Units Produced</t>
   </si>
@@ -95,6 +95,54 @@
   <si>
     <t>Percentiles grouped data:</t>
   </si>
+  <si>
+    <t>5.00 under 5.50</t>
+  </si>
+  <si>
+    <t>5.50 under 6.00</t>
+  </si>
+  <si>
+    <t>6.00 under 6.50</t>
+  </si>
+  <si>
+    <t>6.50 under 7.00</t>
+  </si>
+  <si>
+    <t>7.00 under 7.50</t>
+  </si>
+  <si>
+    <t>7.50 under 8.00</t>
+  </si>
+  <si>
+    <t>8.00 under 8.50</t>
+  </si>
+  <si>
+    <t>8.50 under 9.00</t>
+  </si>
+  <si>
+    <t>9.00 under 9.50</t>
+  </si>
+  <si>
+    <t>average:</t>
+  </si>
+  <si>
+    <t>median:</t>
+  </si>
+  <si>
+    <t>rel freq</t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>total units:</t>
+  </si>
 </sst>
 </file>
 
@@ -137,9 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,7 +310,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$J$9:$J$16</c:f>
+              <c:f>intro!$J$9:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -292,7 +343,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$9:$K$16</c:f>
+              <c:f>intro!$K$9:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -591,7 +642,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$N$9:$N$16</c:f>
+              <c:f>intro!$N$9:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -624,7 +675,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$9:$O$16</c:f>
+              <c:f>intro!$O$9:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -917,7 +968,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$9:$E$15</c:f>
+              <c:f>intro!$E$9:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -947,7 +998,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$9:$G$15</c:f>
+              <c:f>intro!$G$9:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1146,6 +1197,341 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Histogram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'3.2_#6'!$D$1:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3.2_#6'!$E$1:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F7F3-433E-BC5F-CCF07D8F113B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:overlap val="-27"/>
+        <c:axId val="422057504"/>
+        <c:axId val="422058160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="422057504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422058160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="422058160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422057504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1266,6 +1652,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2299,6 +2725,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2914,6 +3843,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3F7F91-E460-46C9-9049-C3A38EB3899B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.36833</cdr:x>
+      <cdr:y>0.24514</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.46792</cdr:x>
+      <cdr:y>0.42847</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB09DB99-BBCA-4785-92EE-669AC989317B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1684020" y="672465"/>
+          <a:ext cx="455295" cy="502920"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.36792</cdr:x>
+      <cdr:y>0.24375</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.46833</cdr:x>
+      <cdr:y>0.38681</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BF60859-E19D-4C63-AD17-FECF2F18A06B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="1682115" y="668655"/>
+          <a:ext cx="459105" cy="392430"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.4111</cdr:x>
+      <cdr:y>0.24482</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41504</cdr:x>
+      <cdr:y>0.88565</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6D8872A-C404-409F-90E7-4AA8E4F107DB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1879554" y="671582"/>
+          <a:ext cx="18029" cy="1757922"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3179,13 +4289,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3832,8 +4943,8 @@
         <v>50</v>
       </c>
       <c r="I33">
-        <f>190+10*((($G$16*80)/100-K13)/G12)</f>
-        <v>196.22222222222223</v>
+        <f>190+10*((($G$16*50)/100-K12)/G12)</f>
+        <v>195.55555555555554</v>
       </c>
     </row>
   </sheetData>
@@ -3843,4 +4954,370 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1">
+        <v>5.49</v>
+      </c>
+      <c r="D1">
+        <v>5.25</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <f>D1*E1</f>
+        <v>26.25</v>
+      </c>
+      <c r="G1" s="1">
+        <f>E1/$E$11</f>
+        <v>2.2727272727272728E-2</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1">
+        <v>5.5</v>
+      </c>
+      <c r="J1">
+        <f>5</f>
+        <v>5</v>
+      </c>
+      <c r="K1" s="1">
+        <f>J1/$E$11</f>
+        <v>2.2727272727272728E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>5.99</v>
+      </c>
+      <c r="D2">
+        <v>5.75</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2</f>
+        <v>126.5</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2/$E$11</f>
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <f>J1+E2</f>
+        <v>27</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K9" si="0">J2/$E$11</f>
+        <v>0.12272727272727273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>6.49</v>
+      </c>
+      <c r="D3">
+        <v>6.25</v>
+      </c>
+      <c r="E3">
+        <v>49</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="1">D3*E3</f>
+        <v>306.25</v>
+      </c>
+      <c r="G3" s="1">
+        <f>E3/$E$11</f>
+        <v>0.22272727272727272</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3">
+        <v>6.5</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J9" si="2">J2+E3</f>
+        <v>76</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.34545454545454546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>6.99</v>
+      </c>
+      <c r="D4">
+        <v>6.75</v>
+      </c>
+      <c r="E4">
+        <v>63</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>425.25</v>
+      </c>
+      <c r="G4" s="1">
+        <f>E4/$E$11</f>
+        <v>0.28636363636363638</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63181818181818183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>7.49</v>
+      </c>
+      <c r="D5">
+        <v>7.25</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>326.25</v>
+      </c>
+      <c r="G5" s="1">
+        <f>E5/$E$11</f>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5">
+        <v>7.5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83636363636363631</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>7.99</v>
+      </c>
+      <c r="D6">
+        <v>7.75</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>193.75</v>
+      </c>
+      <c r="G6" s="1">
+        <f>E6/$E$11</f>
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>8.49</v>
+      </c>
+      <c r="D7">
+        <v>8.25</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>41.25</v>
+      </c>
+      <c r="G7" s="1">
+        <f>E7/$E$11</f>
+        <v>2.2727272727272728E-2</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7">
+        <v>8.5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>214</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.97272727272727277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>8.99</v>
+      </c>
+      <c r="D8">
+        <v>8.75</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="G8" s="1">
+        <f>E8/$E$11</f>
+        <v>1.8181818181818181E-2</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>218</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.99090909090909096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>9.49</v>
+      </c>
+      <c r="D9">
+        <v>9.25</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>18.5</v>
+      </c>
+      <c r="G9" s="1">
+        <f>E9/$E$11</f>
+        <v>9.0909090909090905E-3</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9">
+        <v>9.5</v>
+      </c>
+      <c r="J9">
+        <f>J8+E9</f>
+        <v>220</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E1:E9)</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <f>SUM(F1:F9)/SUM(E1:E9)</f>
+        <v>6.8136363636363635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <f>6.5+0.5*(((E11*50)/100-J3)/E4)</f>
+        <v>6.7698412698412698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>